<commit_message>
remove property source duplicated file
</commit_message>
<xml_diff>
--- a/legislator/property/output/normal/林佳龍_2012-04-09_財產申報表_tmpf4911.xlsx
+++ b/legislator/property/output/normal/林佳龍_2012-04-09_財產申報表_tmpf4911.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="128">
   <si>
     <t>name</t>
   </si>
@@ -259,9 +259,6 @@
     <t>三商美邦人壽</t>
   </si>
   <si>
-    <t>二商美邦人壽</t>
-  </si>
-  <si>
     <t>國際紐約人壽</t>
   </si>
   <si>
@@ -280,7 +277,7 @@
     <t>15年繳費金富多终身保險</t>
   </si>
   <si>
-    <t>永安終身壽險主約:I£OM005886</t>
+    <t>永安終身壽險主約:LBOM005886</t>
   </si>
   <si>
     <t>永安终身壽險(附約）</t>
@@ -898,7 +895,7 @@
         <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -939,22 +936,22 @@
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="2">
         <v>45579600</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>23</v>
@@ -983,22 +980,22 @@
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="2">
         <v>100</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
@@ -1027,22 +1024,22 @@
         <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" s="2">
         <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>23</v>
@@ -1071,22 +1068,22 @@
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="2">
         <v>100</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>
@@ -1115,22 +1112,22 @@
         <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>23</v>
@@ -1159,22 +1156,22 @@
         <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2">
         <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>23</v>
@@ -2846,13 +2843,13 @@
         <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>23</v>
@@ -2881,13 +2878,13 @@
         <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>23</v>
@@ -2916,13 +2913,13 @@
         <v>77</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>23</v>
@@ -2951,13 +2948,13 @@
         <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>23</v>
@@ -2986,13 +2983,13 @@
         <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -3018,16 +3015,16 @@
         <v>111</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>23</v>
@@ -3053,16 +3050,16 @@
         <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>23</v>
@@ -3088,16 +3085,16 @@
         <v>113</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>23</v>
@@ -3123,16 +3120,16 @@
         <v>114</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>23</v>
@@ -3158,16 +3155,16 @@
         <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>23</v>
@@ -3193,16 +3190,16 @@
         <v>116</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>23</v>
@@ -3228,16 +3225,16 @@
         <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
@@ -3263,16 +3260,16 @@
         <v>118</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>23</v>
@@ -3298,16 +3295,16 @@
         <v>120</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>23</v>
@@ -3333,16 +3330,16 @@
         <v>121</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>23</v>
@@ -3368,16 +3365,16 @@
         <v>122</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>23</v>
@@ -3403,16 +3400,16 @@
         <v>123</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>23</v>
@@ -3438,16 +3435,16 @@
         <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>23</v>
@@ -3473,16 +3470,16 @@
         <v>125</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>23</v>
@@ -3508,16 +3505,16 @@
         <v>126</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>23</v>
@@ -3543,16 +3540,16 @@
         <v>127</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>23</v>
@@ -3578,16 +3575,16 @@
         <v>128</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>23</v>
@@ -3613,16 +3610,16 @@
         <v>129</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>23</v>
@@ -3648,16 +3645,16 @@
         <v>130</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>23</v>
@@ -3683,16 +3680,16 @@
         <v>131</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>23</v>
@@ -3718,16 +3715,16 @@
         <v>132</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>23</v>
@@ -3753,16 +3750,16 @@
         <v>133</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>23</v>
@@ -3788,16 +3785,16 @@
         <v>134</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>23</v>
@@ -3823,16 +3820,16 @@
         <v>135</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>23</v>
@@ -3858,16 +3855,16 @@
         <v>136</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>23</v>
@@ -3893,16 +3890,16 @@
         <v>137</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>23</v>
@@ -3928,16 +3925,16 @@
         <v>138</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>23</v>
@@ -3963,16 +3960,16 @@
         <v>139</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>23</v>
@@ -3998,16 +3995,16 @@
         <v>140</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>23</v>
@@ -4033,16 +4030,16 @@
         <v>141</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>23</v>
@@ -4068,16 +4065,16 @@
         <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>23</v>
@@ -4103,16 +4100,16 @@
         <v>144</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>23</v>
@@ -4138,16 +4135,16 @@
         <v>145</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>23</v>
@@ -4183,13 +4180,13 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -4227,25 +4224,25 @@
         <v>150</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E2" s="2">
         <v>97331145</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>23</v>
@@ -4271,25 +4268,25 @@
         <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="E3" s="2">
         <v>19154</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
@@ -4325,10 +4322,10 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -4369,25 +4366,25 @@
         <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="2">
         <v>24198509</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>23</v>
@@ -4413,7 +4410,7 @@
         <v>157</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
@@ -4425,13 +4422,13 @@
         <v>7662466</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
@@ -4457,25 +4454,25 @@
         <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2">
         <v>6231419</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>23</v>
@@ -4501,25 +4498,25 @@
         <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="2">
         <v>941036</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>23</v>

</xml_diff>